<commit_message>
Added working thesis PDF thing.
</commit_message>
<xml_diff>
--- a/data/Keywords.xlsx
+++ b/data/Keywords.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\School\BachelorThesis\ArchitecturalKnowledgeResearch\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C09FF59-9659-4766-843E-3B30DEF2E79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20580" windowHeight="9470"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,13 +54,13 @@
     <t>advantag* alternativ* appropriate assum* benefit* better best caus* choic* choos* complex* condition* critical decid* decision* eas* evaluat* hard* quick* rational* reason* risk* simpl* strong* tradeoff weak* rational* disadvantag* comparison* pros cons good differen* slow* lightweight overkill* recommend* suggest* propos* outperform* important* versus vs contrast* distinct* fast* heav* boost* drawback* option*</t>
   </si>
   <si>
-    <t>Reusbale Solutions</t>
+    <t>Reusable Solutions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,20 +396,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="153.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -424,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -432,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -440,7 +441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Added ak-tagger as a better way to query, tag, and share tagged data.
</commit_message>
<xml_diff>
--- a/data/Keywords.xlsx
+++ b/data/Keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\School\BachelorThesis\ArchitecturalKnowledgeResearch\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78FA633-C150-4CFA-94CC-0F963ED8D8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A33BF0B-DF21-4466-8722-A45418A5AFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>